<commit_message>
corrigiendo error de subgrupos
</commit_message>
<xml_diff>
--- a/servicios/export.xlsx
+++ b/servicios/export.xlsx
@@ -17,12 +17,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
-    <t xml:space="preserve">Falabella (Chile+CMR) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cencosud (Paris+Mas) </t>
-  </si>
-  <si>
     <t>Ripley Chile</t>
   </si>
   <si>
@@ -33,6 +27,12 @@
   </si>
   <si>
     <t>Hites</t>
+  </si>
+  <si>
+    <t>Falabella Chile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paris Chile  </t>
   </si>
   <si>
     <t>Q1</t>
@@ -117,7 +117,7 @@
               <a:rPr b="0" i="0" u="none" strike="noStrike">
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Test Grouped Column Chart</a:t>
+              <a:t>Grafico</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -141,7 +141,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Falabella (Chile+CMR) </c:v>
+                  <c:v>Ripley Chile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -230,40 +230,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>233542</c:v>
+                  <c:v>10.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>254770</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>246159</c:v>
+                  <c:v>17.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>313263</c:v>
+                  <c:v>14.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>239524</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>298623</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>275302</c:v>
+                  <c:v>5.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>374579</c:v>
+                  <c:v>8.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>282887</c:v>
+                  <c:v>9.3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>323310</c:v>
+                  <c:v>7.2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>302521</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>395808</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -278,7 +278,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cencosud (Paris+Mas) </c:v>
+                  <c:v>ABCDIN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -290,40 +290,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>167280</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>177713</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>168046</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>232725</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>162751</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>206590</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>190009</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>256034</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>197796</c:v>
+                  <c:v>10.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>227685</c:v>
+                  <c:v>8.9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>211603</c:v>
+                  <c:v>15.9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>276250</c:v>
+                  <c:v>16.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -338,7 +338,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ripley Chile</c:v>
+                  <c:v>La Polar Chile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -350,40 +350,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>153558</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>163183</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>149899</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>204105</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>146943</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>185685</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>168268</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>230886</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>171694</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>194699</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>175379</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>240846</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -398,7 +398,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ABCDIN</c:v>
+                  <c:v>Hites</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -410,40 +410,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>39.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>25.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>30.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46561</c:v>
+                  <c:v>29.4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60811</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>66874</c:v>
+                  <c:v>14.9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>68830</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>60297</c:v>
+                  <c:v>9.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>71891</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>59426</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>83423</c:v>
+                  <c:v>-0.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -458,7 +458,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>La Polar Chile</c:v>
+                  <c:v>Falabella Chile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -470,40 +470,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>26.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>15.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>18.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>20.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>9.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>9.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>-0.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>104093</c:v>
+                  <c:v>-0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -518,7 +518,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hites</c:v>
+                  <c:v>Paris Chile  </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -530,40 +530,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>29510</c:v>
+                  <c:v>11.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35315</c:v>
+                  <c:v>30.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32630</c:v>
+                  <c:v>22.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48906</c:v>
+                  <c:v>15.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32223</c:v>
+                  <c:v>17.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45917</c:v>
+                  <c:v>-1.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41370</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64401</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42968</c:v>
+                  <c:v>9.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54256</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>53014</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>77275</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1001,7 +1001,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1037,22 +1037,22 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>233542</v>
+        <v>10.6</v>
       </c>
       <c r="D2">
-        <v>167280</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>153558</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="H2">
-        <v>29510</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1060,22 +1060,22 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>254770</v>
+        <v>28.5</v>
       </c>
       <c r="D3">
-        <v>177713</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>163183</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>39.8</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>26.2</v>
       </c>
       <c r="H3">
-        <v>35315</v>
+        <v>30.8</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1083,22 +1083,22 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>246159</v>
+        <v>17.4</v>
       </c>
       <c r="D4">
-        <v>168046</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>149899</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>25.8</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>15.6</v>
       </c>
       <c r="H4">
-        <v>32630</v>
+        <v>22.4</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1106,22 +1106,22 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>313263</v>
+        <v>14.2</v>
       </c>
       <c r="D5">
-        <v>232725</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>204105</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>30.6</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>18.9</v>
       </c>
       <c r="H5">
-        <v>48906</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1132,22 +1132,22 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>239524</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>162751</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>146943</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>46561</v>
+        <v>29.4</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>20.9</v>
       </c>
       <c r="H6">
-        <v>32223</v>
+        <v>17.9</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1155,22 +1155,22 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>298623</v>
+        <v>1.5</v>
       </c>
       <c r="D7">
-        <v>206590</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>185685</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>60811</v>
+        <v>9.6</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>3.7</v>
       </c>
       <c r="H7">
-        <v>45917</v>
+        <v>-1.9</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1178,22 +1178,22 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>275302</v>
+        <v>5.3</v>
       </c>
       <c r="D8">
-        <v>190009</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>168268</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>66874</v>
+        <v>14.9</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>9.1</v>
       </c>
       <c r="H8">
-        <v>41370</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1201,22 +1201,22 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>374579</v>
+        <v>8.4</v>
       </c>
       <c r="D9">
-        <v>256034</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>230886</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>68830</v>
+        <v>9.5</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>5.6</v>
       </c>
       <c r="H9">
-        <v>64401</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1227,22 +1227,22 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <v>282887</v>
+        <v>9.3</v>
       </c>
       <c r="D10">
-        <v>197796</v>
+        <v>10.1</v>
       </c>
       <c r="E10">
-        <v>171694</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>60297</v>
+        <v>9.1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>9.2</v>
       </c>
       <c r="H10">
-        <v>42968</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1250,22 +1250,22 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>323310</v>
+        <v>7.2</v>
       </c>
       <c r="D11">
-        <v>227685</v>
+        <v>8.9</v>
       </c>
       <c r="E11">
-        <v>194699</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>71891</v>
+        <v>1.7</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="H11">
-        <v>54256</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1273,22 +1273,22 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <v>302521</v>
+        <v>9.9</v>
       </c>
       <c r="D12">
-        <v>211603</v>
+        <v>15.9</v>
       </c>
       <c r="E12">
-        <v>175379</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>59426</v>
+        <v>3</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="H12">
-        <v>53014</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1296,22 +1296,22 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>395808</v>
+        <v>7.6</v>
       </c>
       <c r="D13">
-        <v>276250</v>
+        <v>16.3</v>
       </c>
       <c r="E13">
-        <v>240846</v>
+        <v>15</v>
       </c>
       <c r="F13">
-        <v>83423</v>
+        <v>-0.2</v>
       </c>
       <c r="G13">
-        <v>104093</v>
+        <v>-0.1</v>
       </c>
       <c r="H13">
-        <v>77275</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1322,22 +1322,22 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <v>320630</v>
+        <v>0.1</v>
       </c>
       <c r="D14">
-        <v>243087</v>
+        <v>15.9</v>
       </c>
       <c r="E14">
-        <v>181959</v>
+        <v>15</v>
       </c>
       <c r="F14">
-        <v>68002</v>
+        <v>3.9</v>
       </c>
       <c r="G14">
-        <v>74686</v>
+        <v>-0.6</v>
       </c>
       <c r="H14">
-        <v>52444</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -1345,22 +1345,22 @@
         <v>7</v>
       </c>
       <c r="C15">
-        <v>333045</v>
+        <v>-3.5</v>
       </c>
       <c r="D15">
-        <v>268116</v>
+        <v>21.4</v>
       </c>
       <c r="E15">
-        <v>196529</v>
+        <v>16</v>
       </c>
       <c r="F15">
-        <v>72012</v>
+        <v>7</v>
       </c>
       <c r="G15">
-        <v>85098</v>
+        <v>4.7</v>
       </c>
       <c r="H15">
-        <v>62514</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1368,22 +1368,22 @@
         <v>8</v>
       </c>
       <c r="C16">
-        <v>321947</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>260445</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>189933</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>71332</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>80213</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>58831</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1391,22 +1391,22 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>419376</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>338153</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>262762</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>95113</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>111933</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>80041</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1417,22 +1417,45 @@
         <v>6</v>
       </c>
       <c r="C18">
-        <v>340662</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>259031</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>185161</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>75063</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>82991</v>
+        <v>0</v>
       </c>
       <c r="H18">
-        <v>54081</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solo falta agregar empresas extras a la busqueda
</commit_message>
<xml_diff>
--- a/servicios/export.xlsx
+++ b/servicios/export.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">Cencosud (Paris+Mas) </t>
+  </si>
   <si>
     <t>Ripley Chile</t>
   </si>
@@ -35,16 +38,7 @@
     <t xml:space="preserve">Paris Chile  </t>
   </si>
   <si>
-    <t>Q1</t>
-  </si>
-  <si>
     <t>Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>Q4</t>
   </si>
 </sst>
 </file>
@@ -141,7 +135,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ripley Chile</c:v>
+                  <c:v>Cencosud (Paris+Mas) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -152,17 +146,25 @@
               <c:f>Worksheet!$A$2:$B$13</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="2"/>
+                <c:lvl/>
+                <c:lvl/>
+                <c:lvl/>
+                <c:lvl/>
+                <c:lvl/>
+                <c:lvl/>
+                <c:lvl/>
                 <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2013</c:v>
+                  </c:pt>
                   <c:pt idx="1">
-                    <c:v>Q4</c:v>
+                    <c:v>Q2</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
-                  <c:pt idx="1">
-                    <c:v>Q3</c:v>
+                  <c:pt idx="0">
+                    <c:v>2012</c:v>
                   </c:pt>
-                </c:lvl>
-                <c:lvl>
                   <c:pt idx="1">
                     <c:v>Q2</c:v>
                   </c:pt>
@@ -172,21 +174,6 @@
                     <c:v>2011</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Q1</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="1">
-                    <c:v>Q4</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="1">
-                    <c:v>Q3</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="1">
                     <c:v>Q2</c:v>
                   </c:pt>
                 </c:lvl>
@@ -194,21 +181,6 @@
                   <c:pt idx="0">
                     <c:v>2010</c:v>
                   </c:pt>
-                  <c:pt idx="1">
-                    <c:v>Q1</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="1">
-                    <c:v>Q4</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="1">
-                    <c:v>Q3</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
                   <c:pt idx="1">
                     <c:v>Q2</c:v>
                   </c:pt>
@@ -218,7 +190,7 @@
                     <c:v>2009</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Q1</c:v>
+                    <c:v>Q2</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -230,40 +202,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>10.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.3</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.4</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.3</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.2</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.9</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.6</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -278,7 +250,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ABCDIN</c:v>
+                  <c:v>Ripley Chile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -290,40 +262,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>210928</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>532406</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>590032</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>633446</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>680580</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.1</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.9</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.9</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.3</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -338,7 +310,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>La Polar Chile</c:v>
+                  <c:v>ABCDIN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -353,37 +325,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>67931</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>153483</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>173802</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>217986</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -398,7 +370,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hites</c:v>
+                  <c:v>La Polar Chile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -410,40 +382,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.6</c:v>
+                  <c:v>216112</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.4</c:v>
+                  <c:v>311418</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.6</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14.9</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.5</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.1</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.7</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.2</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -458,7 +430,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Falabella Chile</c:v>
+                  <c:v>Hites</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -470,40 +442,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>5.6</c:v>
+                  <c:v>38935</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.2</c:v>
+                  <c:v>103494</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.6</c:v>
+                  <c:v>130372</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.9</c:v>
+                  <c:v>160765</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.9</c:v>
+                  <c:v>171246</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.1</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.2</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.5</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.1</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -518,7 +490,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Paris Chile  </c:v>
+                  <c:v>Falabella Chile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -530,40 +502,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>11.1</c:v>
+                  <c:v>354196</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.8</c:v>
+                  <c:v>847160</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.4</c:v>
+                  <c:v>984150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.4</c:v>
+                  <c:v>1079538</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.9</c:v>
+                  <c:v>1152675</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.9</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.7</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.4</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.5</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.2</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.7</c:v>
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1001,7 +973,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1009,7 +981,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -1028,434 +1000,153 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>2009</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
-        <v>10.6</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>210928</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>5.6</v>
+        <v>38935</v>
       </c>
       <c r="H2">
-        <v>11.1</v>
+        <v>354196</v>
+      </c>
+      <c r="I2">
+        <v>226830</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
+      <c r="A3">
+        <v>2010</v>
+      </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3">
-        <v>28.5</v>
+        <v>0</v>
       </c>
       <c r="D3">
+        <v>532406</v>
+      </c>
+      <c r="E3">
+        <v>67931</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="E3">
+      <c r="G3">
+        <v>103494</v>
+      </c>
+      <c r="H3">
+        <v>847160</v>
+      </c>
+      <c r="I3">
+        <v>564679</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>2011</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>39.8</v>
-      </c>
-      <c r="G3">
-        <v>26.2</v>
-      </c>
-      <c r="H3">
-        <v>30.8</v>
+      <c r="D4">
+        <v>590032</v>
+      </c>
+      <c r="E4">
+        <v>153483</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>130372</v>
+      </c>
+      <c r="H4">
+        <v>984150</v>
+      </c>
+      <c r="I4">
+        <v>656930</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>17.4</v>
-      </c>
-      <c r="D4">
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>2012</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
         <v>0</v>
       </c>
-      <c r="E4">
+      <c r="D5">
+        <v>633446</v>
+      </c>
+      <c r="E5">
+        <v>173802</v>
+      </c>
+      <c r="F5">
+        <v>216112</v>
+      </c>
+      <c r="G5">
+        <v>160765</v>
+      </c>
+      <c r="H5">
+        <v>1079538</v>
+      </c>
+      <c r="I5">
+        <v>777464</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>2013</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>25.8</v>
-      </c>
-      <c r="G4">
-        <v>15.6</v>
-      </c>
-      <c r="H4">
-        <v>22.4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>14.2</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>30.6</v>
-      </c>
-      <c r="G5">
-        <v>18.9</v>
-      </c>
-      <c r="H5">
-        <v>15.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6">
-        <v>2010</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>18</v>
-      </c>
       <c r="D6">
-        <v>0</v>
+        <v>680580</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>217986</v>
       </c>
       <c r="F6">
-        <v>29.4</v>
+        <v>311418</v>
       </c>
       <c r="G6">
-        <v>20.9</v>
+        <v>171246</v>
       </c>
       <c r="H6">
-        <v>17.9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>1.5</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>9.6</v>
-      </c>
-      <c r="G7">
-        <v>3.7</v>
-      </c>
-      <c r="H7">
-        <v>-1.9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8">
-        <v>5.3</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>14.9</v>
-      </c>
-      <c r="G8">
-        <v>9.1</v>
-      </c>
-      <c r="H8">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>8.4</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>9.5</v>
-      </c>
-      <c r="G9">
-        <v>5.6</v>
-      </c>
-      <c r="H9">
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
-        <v>2011</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>9.3</v>
-      </c>
-      <c r="D10">
-        <v>10.1</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>9.1</v>
-      </c>
-      <c r="G10">
-        <v>9.2</v>
-      </c>
-      <c r="H10">
-        <v>9.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11">
-        <v>7.2</v>
-      </c>
-      <c r="D11">
-        <v>8.9</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>1.7</v>
-      </c>
-      <c r="G11">
-        <v>1.6</v>
-      </c>
-      <c r="H11">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12">
-        <v>9.9</v>
-      </c>
-      <c r="D12">
-        <v>15.9</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>-0.5</v>
-      </c>
-      <c r="H12">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13">
-        <v>7.6</v>
-      </c>
-      <c r="D13">
-        <v>16.3</v>
-      </c>
-      <c r="E13">
-        <v>15</v>
-      </c>
-      <c r="F13">
-        <v>-0.2</v>
-      </c>
-      <c r="G13">
-        <v>-0.1</v>
-      </c>
-      <c r="H13">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14">
-        <v>2012</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14">
-        <v>0.1</v>
-      </c>
-      <c r="D14">
-        <v>15.9</v>
-      </c>
-      <c r="E14">
-        <v>15</v>
-      </c>
-      <c r="F14">
-        <v>3.9</v>
-      </c>
-      <c r="G14">
-        <v>-0.6</v>
-      </c>
-      <c r="H14">
-        <v>4.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15">
-        <v>-3.5</v>
-      </c>
-      <c r="D15">
-        <v>21.4</v>
-      </c>
-      <c r="E15">
-        <v>16</v>
-      </c>
-      <c r="F15">
-        <v>7</v>
-      </c>
-      <c r="G15">
-        <v>4.7</v>
-      </c>
-      <c r="H15">
-        <v>2.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="B16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18">
-        <v>2013</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
+        <v>1152675</v>
+      </c>
+      <c r="I6">
+        <v>924158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
preparando exportacion de 3 graficos
</commit_message>
<xml_diff>
--- a/servicios/export.xlsx
+++ b/servicios/export.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+  <si>
+    <t xml:space="preserve">Falabella (Chile+CMR) </t>
+  </si>
   <si>
     <t xml:space="preserve">Cencosud (Paris+Mas) </t>
   </si>
@@ -32,13 +35,70 @@
     <t>Hites</t>
   </si>
   <si>
-    <t>Falabella Chile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paris Chile  </t>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>3/2009</t>
   </si>
   <si>
     <t>Q2</t>
+  </si>
+  <si>
+    <t>6/2009</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>9/2009</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>12/2009</t>
+  </si>
+  <si>
+    <t>3/2010</t>
+  </si>
+  <si>
+    <t>6/2010</t>
+  </si>
+  <si>
+    <t>9/2010</t>
+  </si>
+  <si>
+    <t>12/2010</t>
+  </si>
+  <si>
+    <t>3/2011</t>
+  </si>
+  <si>
+    <t>6/2011</t>
+  </si>
+  <si>
+    <t>9/2011</t>
+  </si>
+  <si>
+    <t>12/2011</t>
+  </si>
+  <si>
+    <t>3/2012</t>
+  </si>
+  <si>
+    <t>6/2012</t>
+  </si>
+  <si>
+    <t>9/2012</t>
+  </si>
+  <si>
+    <t>12/2012</t>
+  </si>
+  <si>
+    <t>3/2013</t>
+  </si>
+  <si>
+    <t>6/2013</t>
   </si>
 </sst>
 </file>
@@ -135,7 +195,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cencosud (Paris+Mas) </c:v>
+                  <c:v>Falabella (Chile+CMR) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -146,25 +206,17 @@
               <c:f>Worksheet!$A$2:$B$13</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="2"/>
-                <c:lvl/>
-                <c:lvl/>
-                <c:lvl/>
-                <c:lvl/>
-                <c:lvl/>
-                <c:lvl/>
-                <c:lvl/>
                 <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2013</c:v>
-                  </c:pt>
                   <c:pt idx="1">
-                    <c:v>Q2</c:v>
+                    <c:v>Q4</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2012</c:v>
+                  <c:pt idx="1">
+                    <c:v>Q3</c:v>
                   </c:pt>
+                </c:lvl>
+                <c:lvl>
                   <c:pt idx="1">
                     <c:v>Q2</c:v>
                   </c:pt>
@@ -174,6 +226,21 @@
                     <c:v>2011</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q4</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
                     <c:v>Q2</c:v>
                   </c:pt>
                 </c:lvl>
@@ -181,6 +248,21 @@
                   <c:pt idx="0">
                     <c:v>2010</c:v>
                   </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q4</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
                   <c:pt idx="1">
                     <c:v>Q2</c:v>
                   </c:pt>
@@ -190,7 +272,7 @@
                     <c:v>2009</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Q2</c:v>
+                    <c:v>Q1</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -202,40 +284,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>233542</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>254770</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>246159</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>313263</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>239524</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>298623</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>275302</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>374579</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>282887</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>323310</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v/>
+                  <c:v>302521</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v/>
+                  <c:v>395808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -250,7 +332,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ripley Chile</c:v>
+                  <c:v>Cencosud (Paris+Mas) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -262,40 +344,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>210928</c:v>
+                  <c:v>167280</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>532406</c:v>
+                  <c:v>177713</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>590032</c:v>
+                  <c:v>168046</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>633446</c:v>
+                  <c:v>232725</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>680580</c:v>
+                  <c:v>162751</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>206590</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>190009</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>256034</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>197796</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>227685</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v/>
+                  <c:v>211603</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v/>
+                  <c:v>276250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -310,7 +392,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ABCDIN</c:v>
+                  <c:v>Ripley Chile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -322,40 +404,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>153558</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67931</c:v>
+                  <c:v>163183</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>153483</c:v>
+                  <c:v>149899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>173802</c:v>
+                  <c:v>204105</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>217986</c:v>
+                  <c:v>146943</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>185685</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>168268</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>230886</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>171694</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>194699</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v/>
+                  <c:v>175379</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v/>
+                  <c:v>240846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -370,7 +452,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>La Polar Chile</c:v>
+                  <c:v>ABCDIN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -391,31 +473,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>216112</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>311418</c:v>
+                  <c:v>46561</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>60811</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>66874</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>68830</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>60297</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>71891</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v/>
+                  <c:v>59426</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v/>
+                  <c:v>83423</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -430,7 +512,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hites</c:v>
+                  <c:v>La Polar Chile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -442,40 +524,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>38935</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>103494</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>130372</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160765</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>171246</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v/>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v/>
+                  <c:v>104093</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -490,7 +572,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Falabella Chile</c:v>
+                  <c:v>Hites</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -502,40 +584,40 @@
               <c:numCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>354196</c:v>
+                  <c:v>29510</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>847160</c:v>
+                  <c:v>35315</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>984150</c:v>
+                  <c:v>32630</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1079538</c:v>
+                  <c:v>48906</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1152675</c:v>
+                  <c:v>32223</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v/>
+                  <c:v>45917</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>41370</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v/>
+                  <c:v>64401</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v/>
+                  <c:v>42968</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v/>
+                  <c:v>54256</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v/>
+                  <c:v>53014</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v/>
+                  <c:v>77275</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -973,7 +1055,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -981,7 +1063,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:16">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -1000,153 +1082,830 @@
       <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
-        <v>6</v>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>2009</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>233542</v>
+      </c>
+      <c r="D2">
+        <v>167280</v>
+      </c>
+      <c r="E2">
+        <v>153558</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>29510</v>
+      </c>
+      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>210928</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>38935</v>
-      </c>
-      <c r="H2">
-        <v>354196</v>
-      </c>
-      <c r="I2">
-        <v>226830</v>
+      <c r="K2">
+        <v>233542</v>
+      </c>
+      <c r="L2">
+        <v>167280</v>
+      </c>
+      <c r="M2">
+        <v>153558</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>29510</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3">
+    <row r="3" spans="1:16">
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>254770</v>
+      </c>
+      <c r="D3">
+        <v>177713</v>
+      </c>
+      <c r="E3">
+        <v>163183</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>35315</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3">
+        <v>254770</v>
+      </c>
+      <c r="L3">
+        <v>177713</v>
+      </c>
+      <c r="M3">
+        <v>163183</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>35315</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>246159</v>
+      </c>
+      <c r="D4">
+        <v>168046</v>
+      </c>
+      <c r="E4">
+        <v>149899</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>32630</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4">
+        <v>246159</v>
+      </c>
+      <c r="L4">
+        <v>168046</v>
+      </c>
+      <c r="M4">
+        <v>149899</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>32630</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>313263</v>
+      </c>
+      <c r="D5">
+        <v>232725</v>
+      </c>
+      <c r="E5">
+        <v>204105</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>48906</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5">
+        <v>313263</v>
+      </c>
+      <c r="L5">
+        <v>232725</v>
+      </c>
+      <c r="M5">
+        <v>204105</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>48906</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6">
         <v>2010</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>532406</v>
-      </c>
-      <c r="E3">
-        <v>67931</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>103494</v>
-      </c>
-      <c r="H3">
-        <v>847160</v>
-      </c>
-      <c r="I3">
-        <v>564679</v>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>239524</v>
+      </c>
+      <c r="D6">
+        <v>162751</v>
+      </c>
+      <c r="E6">
+        <v>146943</v>
+      </c>
+      <c r="F6">
+        <v>46561</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>32223</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6">
+        <v>239524</v>
+      </c>
+      <c r="L6">
+        <v>162751</v>
+      </c>
+      <c r="M6">
+        <v>146943</v>
+      </c>
+      <c r="N6">
+        <v>46561</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>32223</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4">
+    <row r="7" spans="1:16">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>298623</v>
+      </c>
+      <c r="D7">
+        <v>206590</v>
+      </c>
+      <c r="E7">
+        <v>185685</v>
+      </c>
+      <c r="F7">
+        <v>60811</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>45917</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7">
+        <v>298623</v>
+      </c>
+      <c r="L7">
+        <v>206590</v>
+      </c>
+      <c r="M7">
+        <v>185685</v>
+      </c>
+      <c r="N7">
+        <v>60811</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>45917</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>275302</v>
+      </c>
+      <c r="D8">
+        <v>190009</v>
+      </c>
+      <c r="E8">
+        <v>168268</v>
+      </c>
+      <c r="F8">
+        <v>66874</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>41370</v>
+      </c>
+      <c r="J8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8">
+        <v>275302</v>
+      </c>
+      <c r="L8">
+        <v>190009</v>
+      </c>
+      <c r="M8">
+        <v>168268</v>
+      </c>
+      <c r="N8">
+        <v>66874</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>41370</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>374579</v>
+      </c>
+      <c r="D9">
+        <v>256034</v>
+      </c>
+      <c r="E9">
+        <v>230886</v>
+      </c>
+      <c r="F9">
+        <v>68830</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>64401</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9">
+        <v>374579</v>
+      </c>
+      <c r="L9">
+        <v>256034</v>
+      </c>
+      <c r="M9">
+        <v>230886</v>
+      </c>
+      <c r="N9">
+        <v>68830</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>64401</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10">
         <v>2011</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>590032</v>
-      </c>
-      <c r="E4">
-        <v>153483</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>130372</v>
-      </c>
-      <c r="H4">
-        <v>984150</v>
-      </c>
-      <c r="I4">
-        <v>656930</v>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>282887</v>
+      </c>
+      <c r="D10">
+        <v>197796</v>
+      </c>
+      <c r="E10">
+        <v>171694</v>
+      </c>
+      <c r="F10">
+        <v>60297</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>42968</v>
+      </c>
+      <c r="J10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10">
+        <v>282887</v>
+      </c>
+      <c r="L10">
+        <v>197796</v>
+      </c>
+      <c r="M10">
+        <v>171694</v>
+      </c>
+      <c r="N10">
+        <v>60297</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>42968</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
+    <row r="11" spans="1:16">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>323310</v>
+      </c>
+      <c r="D11">
+        <v>227685</v>
+      </c>
+      <c r="E11">
+        <v>194699</v>
+      </c>
+      <c r="F11">
+        <v>71891</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>54256</v>
+      </c>
+      <c r="J11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11">
+        <v>323310</v>
+      </c>
+      <c r="L11">
+        <v>227685</v>
+      </c>
+      <c r="M11">
+        <v>194699</v>
+      </c>
+      <c r="N11">
+        <v>71891</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>54256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>302521</v>
+      </c>
+      <c r="D12">
+        <v>211603</v>
+      </c>
+      <c r="E12">
+        <v>175379</v>
+      </c>
+      <c r="F12">
+        <v>59426</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>53014</v>
+      </c>
+      <c r="J12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12">
+        <v>302521</v>
+      </c>
+      <c r="L12">
+        <v>211603</v>
+      </c>
+      <c r="M12">
+        <v>175379</v>
+      </c>
+      <c r="N12">
+        <v>59426</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>53014</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>395808</v>
+      </c>
+      <c r="D13">
+        <v>276250</v>
+      </c>
+      <c r="E13">
+        <v>240846</v>
+      </c>
+      <c r="F13">
+        <v>83423</v>
+      </c>
+      <c r="G13">
+        <v>104093</v>
+      </c>
+      <c r="H13">
+        <v>77275</v>
+      </c>
+      <c r="J13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13">
+        <v>395808</v>
+      </c>
+      <c r="L13">
+        <v>276250</v>
+      </c>
+      <c r="M13">
+        <v>240846</v>
+      </c>
+      <c r="N13">
+        <v>83423</v>
+      </c>
+      <c r="O13">
+        <v>104093</v>
+      </c>
+      <c r="P13">
+        <v>77275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14">
         <v>2012</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>633446</v>
-      </c>
-      <c r="E5">
-        <v>173802</v>
-      </c>
-      <c r="F5">
-        <v>216112</v>
-      </c>
-      <c r="G5">
-        <v>160765</v>
-      </c>
-      <c r="H5">
-        <v>1079538</v>
-      </c>
-      <c r="I5">
-        <v>777464</v>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>332573</v>
+      </c>
+      <c r="D14">
+        <v>243087</v>
+      </c>
+      <c r="E14">
+        <v>181959</v>
+      </c>
+      <c r="F14">
+        <v>68002</v>
+      </c>
+      <c r="G14">
+        <v>74686</v>
+      </c>
+      <c r="H14">
+        <v>52444</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14">
+        <v>332573</v>
+      </c>
+      <c r="L14">
+        <v>243087</v>
+      </c>
+      <c r="M14">
+        <v>181959</v>
+      </c>
+      <c r="N14">
+        <v>68002</v>
+      </c>
+      <c r="O14">
+        <v>74686</v>
+      </c>
+      <c r="P14">
+        <v>52444</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6">
+    <row r="15" spans="1:16">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>343868</v>
+      </c>
+      <c r="D15">
+        <v>268116</v>
+      </c>
+      <c r="E15">
+        <v>196529</v>
+      </c>
+      <c r="F15">
+        <v>72012</v>
+      </c>
+      <c r="G15">
+        <v>85098</v>
+      </c>
+      <c r="H15">
+        <v>62514</v>
+      </c>
+      <c r="J15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15">
+        <v>343868</v>
+      </c>
+      <c r="L15">
+        <v>268116</v>
+      </c>
+      <c r="M15">
+        <v>196529</v>
+      </c>
+      <c r="N15">
+        <v>72012</v>
+      </c>
+      <c r="O15">
+        <v>85098</v>
+      </c>
+      <c r="P15">
+        <v>62514</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>321947</v>
+      </c>
+      <c r="D16">
+        <v>260445</v>
+      </c>
+      <c r="E16">
+        <v>189933</v>
+      </c>
+      <c r="F16">
+        <v>71332</v>
+      </c>
+      <c r="G16">
+        <v>80213</v>
+      </c>
+      <c r="H16">
+        <v>58831</v>
+      </c>
+      <c r="J16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16">
+        <v>321947</v>
+      </c>
+      <c r="L16">
+        <v>260445</v>
+      </c>
+      <c r="M16">
+        <v>189933</v>
+      </c>
+      <c r="N16">
+        <v>71332</v>
+      </c>
+      <c r="O16">
+        <v>80213</v>
+      </c>
+      <c r="P16">
+        <v>58831</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>419376</v>
+      </c>
+      <c r="D17">
+        <v>338153</v>
+      </c>
+      <c r="E17">
+        <v>262762</v>
+      </c>
+      <c r="F17">
+        <v>95113</v>
+      </c>
+      <c r="G17">
+        <v>111933</v>
+      </c>
+      <c r="H17">
+        <v>80041</v>
+      </c>
+      <c r="J17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17">
+        <v>419376</v>
+      </c>
+      <c r="L17">
+        <v>338153</v>
+      </c>
+      <c r="M17">
+        <v>262762</v>
+      </c>
+      <c r="N17">
+        <v>95113</v>
+      </c>
+      <c r="O17">
+        <v>111933</v>
+      </c>
+      <c r="P17">
+        <v>80041</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18">
         <v>2013</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>680580</v>
-      </c>
-      <c r="E6">
-        <v>217986</v>
-      </c>
-      <c r="F6">
-        <v>311418</v>
-      </c>
-      <c r="G6">
-        <v>171246</v>
-      </c>
-      <c r="H6">
-        <v>1152675</v>
-      </c>
-      <c r="I6">
-        <v>924158</v>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>340662</v>
+      </c>
+      <c r="D18">
+        <v>259031</v>
+      </c>
+      <c r="E18">
+        <v>185161</v>
+      </c>
+      <c r="F18">
+        <v>75063</v>
+      </c>
+      <c r="G18">
+        <v>82991</v>
+      </c>
+      <c r="H18">
+        <v>54081</v>
+      </c>
+      <c r="J18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18">
+        <v>340662</v>
+      </c>
+      <c r="L18">
+        <v>259031</v>
+      </c>
+      <c r="M18">
+        <v>185161</v>
+      </c>
+      <c r="N18">
+        <v>75063</v>
+      </c>
+      <c r="O18">
+        <v>82991</v>
+      </c>
+      <c r="P18">
+        <v>54081</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>366735</v>
+      </c>
+      <c r="D19">
+        <v>283857</v>
+      </c>
+      <c r="E19">
+        <v>201353</v>
+      </c>
+      <c r="F19">
+        <v>91066</v>
+      </c>
+      <c r="G19">
+        <v>97676</v>
+      </c>
+      <c r="H19">
+        <v>66458</v>
+      </c>
+      <c r="J19" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19">
+        <v>366735</v>
+      </c>
+      <c r="L19">
+        <v>283857</v>
+      </c>
+      <c r="M19">
+        <v>201353</v>
+      </c>
+      <c r="N19">
+        <v>91066</v>
+      </c>
+      <c r="O19">
+        <v>97676</v>
+      </c>
+      <c r="P19">
+        <v>66458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
con input complete y corrigiendo division por 0
</commit_message>
<xml_diff>
--- a/servicios/export.xlsx
+++ b/servicios/export.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="IngresosTotales" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="0"/>
@@ -16,6 +16,12 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">Falabella (Chile+CMR) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cencosud (Paris+Mas) </t>
+  </si>
   <si>
     <t>Ripley Chile</t>
   </si>
@@ -27,12 +33,6 @@
   </si>
   <si>
     <t>Hites</t>
-  </si>
-  <si>
-    <t>Falabella Chile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paris Chile  </t>
   </si>
   <si>
     <t>Q1</t>
@@ -117,7 +117,7 @@
               <a:rPr b="0" i="0" u="none" strike="noStrike">
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t>Grafico</a:t>
+              <a:t>Ingresos Totales</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -137,21 +137,62 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Worksheet!$C$1</c:f>
+              <c:f>IngresosTotales!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ripley Chile</c:v>
+                  <c:v>Falabella (Chile+CMR) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="111111"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Worksheet!$A$2:$B$13</c:f>
+              <c:f>IngresosTotales!$A$4:$B$21</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2013</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q4</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2012</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                </c:lvl>
                 <c:lvl>
                   <c:pt idx="1">
                     <c:v>Q4</c:v>
@@ -226,44 +267,62 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Worksheet!$C$2:$C$13</c:f>
+              <c:f>IngresosTotales!$C$4:$C$21</c:f>
               <c:numCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>10.6</c:v>
+                  <c:v>233542</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.5</c:v>
+                  <c:v>254770</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.4</c:v>
+                  <c:v>246159</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.2</c:v>
+                  <c:v>313263</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18</c:v>
+                  <c:v>239524</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5</c:v>
+                  <c:v>298623</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.3</c:v>
+                  <c:v>275302</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.4</c:v>
+                  <c:v>374579</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.3</c:v>
+                  <c:v>282887</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.2</c:v>
+                  <c:v>323310</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.9</c:v>
+                  <c:v>302521</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.6</c:v>
+                  <c:v>395808</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>332573</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>343868</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>321947</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>419376</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>340662</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>366735</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -274,56 +333,79 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Worksheet!$D$1</c:f>
+              <c:f>IngresosTotales!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>ABCDIN</c:v>
+                  <c:v>Cencosud (Paris+Mas) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="222222"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Worksheet!$D$2:$D$13</c:f>
+              <c:f>IngresosTotales!$D$4:$D$21</c:f>
               <c:numCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>167280</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>177713</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>168046</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>232725</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>162751</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>206590</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>190009</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>256034</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.1</c:v>
+                  <c:v>197796</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.9</c:v>
+                  <c:v>227685</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.9</c:v>
+                  <c:v>211603</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16.3</c:v>
+                  <c:v>276250</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>243087</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>268116</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>260445</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>338153</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>259031</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>283857</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -334,56 +416,79 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Worksheet!$E$1</c:f>
+              <c:f>IngresosTotales!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>La Polar Chile</c:v>
+                  <c:v>Ripley Chile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="333333"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Worksheet!$E$2:$E$13</c:f>
+              <c:f>IngresosTotales!$E$4:$E$21</c:f>
               <c:numCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>153558</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>163183</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>149899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>204105</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>146943</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>185685</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>168268</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>230886</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>171694</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>194699</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>175379</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15</c:v>
+                  <c:v>240846</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>181959</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196529</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>189933</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>262762</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>185161</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>201353</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -394,56 +499,79 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Worksheet!$F$1</c:f>
+              <c:f>IngresosTotales!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Hites</c:v>
+                  <c:v>ABCDIN</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="444444"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Worksheet!$F$2:$F$13</c:f>
+              <c:f>IngresosTotales!$F$4:$F$21</c:f>
               <c:numCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>39.8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.4</c:v>
+                  <c:v>46561</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.6</c:v>
+                  <c:v>60811</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14.9</c:v>
+                  <c:v>66874</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.5</c:v>
+                  <c:v>68830</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.1</c:v>
+                  <c:v>60297</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.7</c:v>
+                  <c:v>71891</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>59426</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.2</c:v>
+                  <c:v>83423</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>68002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>72012</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>71332</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>95113</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>75063</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>91066</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -454,56 +582,79 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Worksheet!$G$1</c:f>
+              <c:f>IngresosTotales!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Falabella Chile</c:v>
+                  <c:v>La Polar Chile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="555555"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Worksheet!$G$2:$G$13</c:f>
+              <c:f>IngresosTotales!$G$4:$G$21</c:f>
               <c:numCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>5.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>26.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.1</c:v>
+                  <c:v>104093</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>74686</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>85098</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80213</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>111933</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>82991</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97676</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -514,56 +665,79 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Worksheet!$H$1</c:f>
+              <c:f>IngresosTotales!$H$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Paris Chile  </c:v>
+                  <c:v>Hites</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="666666"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Worksheet!$H$2:$H$13</c:f>
+              <c:f>IngresosTotales!$H$4:$H$21</c:f>
               <c:numCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>11.1</c:v>
+                  <c:v>29510</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.8</c:v>
+                  <c:v>35315</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.4</c:v>
+                  <c:v>32630</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.4</c:v>
+                  <c:v>48906</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17.9</c:v>
+                  <c:v>32223</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-1.9</c:v>
+                  <c:v>45917</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5</c:v>
+                  <c:v>41370</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.7</c:v>
+                  <c:v>64401</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.4</c:v>
+                  <c:v>42968</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.5</c:v>
+                  <c:v>54256</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.2</c:v>
+                  <c:v>53014</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.7</c:v>
+                  <c:v>77275</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>52444</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>62514</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>58831</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80041</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>54081</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>66458</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -630,7 +804,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:r>
-                  <a:t>Value ($k)</a:t>
+                  <a:t>Ingresos Totales</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -666,6 +840,1514 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins footer="0.3" header="0.3" r="0.7" l="0.7" t="0.75" b="0.75"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr b="0" i="0" u="none" strike="noStrike">
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Referente Ingresos Totales</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IngresosTotales!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Falabella (Chile+CMR) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="111111"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>IngresosTotales!$A$25:$B$42</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2013</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q4</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2012</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q4</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2011</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q4</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2010</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q4</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2009</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>IngresosTotales!$C$25:$C$42</c:f>
+              <c:numCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IngresosTotales!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cencosud (Paris+Mas) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="222222"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>IngresosTotales!$D$25:$D$42</c:f>
+              <c:numCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IngresosTotales!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ripley Chile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="333333"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>IngresosTotales!$E$25:$E$42</c:f>
+              <c:numCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IngresosTotales!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ABCDIN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="444444"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>IngresosTotales!$F$25:$F$42</c:f>
+              <c:numCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IngresosTotales!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>La Polar Chile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="555555"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>IngresosTotales!$G$25:$G$42</c:f>
+              <c:numCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IngresosTotales!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hites</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="666666"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>IngresosTotales!$H$25:$H$42</c:f>
+              <c:numCache>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="75091328"/>
+        <c:axId val="75089408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="75091328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:t>Periodo Financiero</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75089408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="75089408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:t>Ingresos Totales</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75089408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins footer="0.3" header="0.3" r="0.7" l="0.7" t="0.75" b="0.75"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr b="0" i="0" u="none" strike="noStrike">
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Variacion Ingresos Totales</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IngresosTotales!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Falabella (Chile+CMR) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="111111"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>IngresosTotales!$A$46:$B$62</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2013</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q4</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2012</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q4</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2011</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q4</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2010</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Q1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q4</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="1">
+                    <c:v>Q3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2009</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Q2</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>IngresosTotales!$C$46:$C$62</c:f>
+              <c:numCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>9.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-23.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-7.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-24.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-6.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-16</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-6.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-18.8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IngresosTotales!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cencosud (Paris+Mas) </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="222222"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>IngresosTotales!$D$46:$D$62</c:f>
+              <c:numCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-30.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-22.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-7.1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30.6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-2.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>29.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-23.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IngresosTotales!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ripley Chile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="333333"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>IngresosTotales!$E$46:$E$62</c:f>
+              <c:numCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-9.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-25.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-9.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-24.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-3.4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>38.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-29.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IngresosTotales!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ABCDIN</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="444444"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>IngresosTotales!$F$46:$F$62</c:f>
+              <c:numCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-12.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-17.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-18.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>33.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-21.1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IngresosTotales!$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>La Polar Chile</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="555555"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>IngresosTotales!$G$46:$G$62</c:f>
+              <c:numCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-28.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-5.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>39.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-25.9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>IngresosTotales!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Hites</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="666666"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>IngresosTotales!$H$46:$H$62</c:f>
+              <c:numCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>19.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-34.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-9.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>55.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-33.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-32.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-5.9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-32.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="75091328"/>
+        <c:axId val="75089408"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="75091328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:t>Periodo Financiero</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75089408"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="75089408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:t>Ingresos Totales</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75089408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:srgbClr val="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins footer="0.3" header="0.3" r="0.7" l="0.7" t="0.75" b="0.75"/>
@@ -678,13 +2360,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -703,6 +2385,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr name="Chart 2" id="2050"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr name="Chart 3" id="3075"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1001,7 +2747,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1009,453 +2755,1328 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="3" spans="1:8">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
+    <row r="4" spans="1:8">
+      <c r="A4">
         <v>2009</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>10.6</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>8</v>
-      </c>
-      <c r="G2">
-        <v>5.6</v>
-      </c>
-      <c r="H2">
-        <v>11.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>28.5</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>39.8</v>
-      </c>
-      <c r="G3">
-        <v>26.2</v>
-      </c>
-      <c r="H3">
-        <v>30.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
       <c r="C4">
-        <v>17.4</v>
+        <v>233542</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>167280</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>153558</v>
       </c>
       <c r="F4">
-        <v>25.8</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>15.6</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>22.4</v>
+        <v>29510</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5">
-        <v>14.2</v>
+        <v>254770</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>177713</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>163183</v>
       </c>
       <c r="F5">
-        <v>30.6</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>18.9</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>15.4</v>
+        <v>35315</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6">
-        <v>2010</v>
-      </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>18</v>
+        <v>246159</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>168046</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>149899</v>
       </c>
       <c r="F6">
-        <v>29.4</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>20.9</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>17.9</v>
+        <v>32630</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="B7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>1.5</v>
+        <v>313263</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>232725</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>204105</v>
       </c>
       <c r="F7">
-        <v>9.6</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>3.7</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>-1.9</v>
+        <v>48906</v>
       </c>
     </row>
     <row r="8" spans="1:8">
+      <c r="A8">
+        <v>2010</v>
+      </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>5.3</v>
+        <v>239524</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>162751</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>146943</v>
       </c>
       <c r="F8">
-        <v>14.9</v>
+        <v>46561</v>
       </c>
       <c r="G8">
-        <v>9.1</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>3.5</v>
+        <v>32223</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>8.4</v>
+        <v>298623</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>206590</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>185685</v>
       </c>
       <c r="F9">
-        <v>9.5</v>
+        <v>60811</v>
       </c>
       <c r="G9">
-        <v>5.6</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>4.7</v>
+        <v>45917</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10">
-        <v>2011</v>
-      </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>9.3</v>
+        <v>275302</v>
       </c>
       <c r="D10">
-        <v>10.1</v>
+        <v>190009</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>168268</v>
       </c>
       <c r="F10">
-        <v>9.1</v>
+        <v>66874</v>
       </c>
       <c r="G10">
-        <v>9.2</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>9.4</v>
+        <v>41370</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="B11" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>7.2</v>
+        <v>374579</v>
       </c>
       <c r="D11">
-        <v>8.9</v>
+        <v>256034</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>230886</v>
       </c>
       <c r="F11">
-        <v>1.7</v>
+        <v>68830</v>
       </c>
       <c r="G11">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>5.5</v>
+        <v>64401</v>
       </c>
     </row>
     <row r="12" spans="1:8">
+      <c r="A12">
+        <v>2011</v>
+      </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12">
-        <v>9.9</v>
+        <v>282887</v>
       </c>
       <c r="D12">
-        <v>15.9</v>
+        <v>197796</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>171694</v>
       </c>
       <c r="F12">
-        <v>3</v>
+        <v>60297</v>
       </c>
       <c r="G12">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>5.2</v>
+        <v>42968</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C13">
-        <v>7.6</v>
+        <v>323310</v>
       </c>
       <c r="D13">
-        <v>16.3</v>
+        <v>227685</v>
       </c>
       <c r="E13">
-        <v>15</v>
+        <v>194699</v>
       </c>
       <c r="F13">
-        <v>-0.2</v>
+        <v>71891</v>
       </c>
       <c r="G13">
-        <v>-0.1</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>2.7</v>
+        <v>54256</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14">
-        <v>2012</v>
-      </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C14">
-        <v>0.1</v>
+        <v>302521</v>
       </c>
       <c r="D14">
-        <v>15.9</v>
+        <v>211603</v>
       </c>
       <c r="E14">
-        <v>15</v>
+        <v>175379</v>
       </c>
       <c r="F14">
-        <v>3.9</v>
+        <v>59426</v>
       </c>
       <c r="G14">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>4.9</v>
+        <v>53014</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C15">
-        <v>-3.5</v>
+        <v>395808</v>
       </c>
       <c r="D15">
-        <v>21.4</v>
+        <v>276250</v>
       </c>
       <c r="E15">
-        <v>16</v>
+        <v>240846</v>
       </c>
       <c r="F15">
-        <v>7</v>
+        <v>83423</v>
       </c>
       <c r="G15">
-        <v>4.7</v>
+        <v>104093</v>
       </c>
       <c r="H15">
-        <v>2.9</v>
+        <v>77275</v>
       </c>
     </row>
     <row r="16" spans="1:8">
+      <c r="A16">
+        <v>2012</v>
+      </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>332573</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>243087</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>181959</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>68002</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>74686</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>52444</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="B17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>343868</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>268116</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>196529</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>72012</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>85098</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>62514</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18">
-        <v>2013</v>
-      </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>321947</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>260445</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>189933</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>71332</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>80213</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>58831</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19">
+        <v>419376</v>
+      </c>
+      <c r="D19">
+        <v>338153</v>
+      </c>
+      <c r="E19">
+        <v>262762</v>
+      </c>
+      <c r="F19">
+        <v>95113</v>
+      </c>
+      <c r="G19">
+        <v>111933</v>
+      </c>
+      <c r="H19">
+        <v>80041</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>2013</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>340662</v>
+      </c>
+      <c r="D20">
+        <v>259031</v>
+      </c>
+      <c r="E20">
+        <v>185161</v>
+      </c>
+      <c r="F20">
+        <v>75063</v>
+      </c>
+      <c r="G20">
+        <v>82991</v>
+      </c>
+      <c r="H20">
+        <v>54081</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="B21" t="s">
         <v>7</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
+      <c r="C21">
+        <v>366735</v>
+      </c>
+      <c r="D21">
+        <v>283857</v>
+      </c>
+      <c r="E21">
+        <v>201353</v>
+      </c>
+      <c r="F21">
+        <v>91066</v>
+      </c>
+      <c r="G21">
+        <v>97676</v>
+      </c>
+      <c r="H21">
+        <v>66458</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>2009</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <v>7.9</v>
+      </c>
+      <c r="D25">
+        <v>5.7</v>
+      </c>
+      <c r="E25">
+        <v>5.2</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="B26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>7.2</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>4.6</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <v>7.5</v>
+      </c>
+      <c r="D27">
+        <v>5.2</v>
+      </c>
+      <c r="E27">
+        <v>4.6</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>6.4</v>
+      </c>
+      <c r="D28">
+        <v>4.8</v>
+      </c>
+      <c r="E28">
+        <v>4.2</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>2010</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>7.4</v>
+      </c>
+      <c r="D29">
+        <v>5.1</v>
+      </c>
+      <c r="E29">
+        <v>4.6</v>
+      </c>
+      <c r="F29">
+        <v>1.4</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>6.5</v>
+      </c>
+      <c r="D30">
+        <v>4.5</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30">
+        <v>1.3</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>6.7</v>
+      </c>
+      <c r="D31">
+        <v>4.6</v>
+      </c>
+      <c r="E31">
+        <v>4.1</v>
+      </c>
+      <c r="F31">
+        <v>1.6</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>5.8</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>3.6</v>
+      </c>
+      <c r="F32">
+        <v>1.1</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>2011</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>6.6</v>
+      </c>
+      <c r="D33">
+        <v>4.6</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>1.4</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>4.2</v>
+      </c>
+      <c r="E34">
+        <v>3.6</v>
+      </c>
+      <c r="F34">
+        <v>1.3</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>5.7</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35">
+        <v>3.3</v>
+      </c>
+      <c r="F35">
+        <v>1.1</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <v>5.1</v>
+      </c>
+      <c r="D36">
+        <v>3.6</v>
+      </c>
+      <c r="E36">
+        <v>3.1</v>
+      </c>
+      <c r="F36">
+        <v>1.1</v>
+      </c>
+      <c r="G36">
+        <v>1.3</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37">
+        <v>2012</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>6.3</v>
+      </c>
+      <c r="D37">
+        <v>4.6</v>
+      </c>
+      <c r="E37">
+        <v>3.5</v>
+      </c>
+      <c r="F37">
+        <v>1.3</v>
+      </c>
+      <c r="G37">
+        <v>1.4</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>5.5</v>
+      </c>
+      <c r="D38">
+        <v>4.3</v>
+      </c>
+      <c r="E38">
+        <v>3.1</v>
+      </c>
+      <c r="F38">
+        <v>1.2</v>
+      </c>
+      <c r="G38">
+        <v>1.4</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39">
+        <v>5.5</v>
+      </c>
+      <c r="D39">
+        <v>4.4</v>
+      </c>
+      <c r="E39">
+        <v>3.2</v>
+      </c>
+      <c r="F39">
+        <v>1.2</v>
+      </c>
+      <c r="G39">
+        <v>1.4</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="B40" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40">
+        <v>5.2</v>
+      </c>
+      <c r="D40">
+        <v>4.2</v>
+      </c>
+      <c r="E40">
+        <v>3.3</v>
+      </c>
+      <c r="F40">
+        <v>1.2</v>
+      </c>
+      <c r="G40">
+        <v>1.4</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41">
+        <v>2013</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41">
+        <v>6.3</v>
+      </c>
+      <c r="D41">
+        <v>4.8</v>
+      </c>
+      <c r="E41">
+        <v>3.4</v>
+      </c>
+      <c r="F41">
+        <v>1.4</v>
+      </c>
+      <c r="G41">
+        <v>1.5</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <v>5.5</v>
+      </c>
+      <c r="D42">
+        <v>4.3</v>
+      </c>
+      <c r="E42">
+        <v>3</v>
+      </c>
+      <c r="F42">
+        <v>1.4</v>
+      </c>
+      <c r="G42">
+        <v>1.5</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="C45" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" t="s">
+        <v>4</v>
+      </c>
+      <c r="H45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46">
+        <v>2009</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46">
+        <v>9.1</v>
+      </c>
+      <c r="D46">
+        <v>6.2</v>
+      </c>
+      <c r="E46">
+        <v>6.3</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="B47" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47">
+        <v>-3.4</v>
+      </c>
+      <c r="D47">
+        <v>-5.4</v>
+      </c>
+      <c r="E47">
+        <v>-8.1</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>-7.6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48">
+        <v>27.3</v>
+      </c>
+      <c r="D48">
+        <v>38.5</v>
+      </c>
+      <c r="E48">
+        <v>36.2</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>49.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49">
+        <v>2010</v>
+      </c>
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49">
+        <v>-23.5</v>
+      </c>
+      <c r="D49">
+        <v>-30.1</v>
+      </c>
+      <c r="E49">
+        <v>-28</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>-34.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50">
+        <v>24.7</v>
+      </c>
+      <c r="D50">
+        <v>26.9</v>
+      </c>
+      <c r="E50">
+        <v>26.4</v>
+      </c>
+      <c r="F50">
+        <v>30.6</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51">
+        <v>-7.8</v>
+      </c>
+      <c r="D51">
+        <v>-8</v>
+      </c>
+      <c r="E51">
+        <v>-9.4</v>
+      </c>
+      <c r="F51">
+        <v>10</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>-9.9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52">
+        <v>36.1</v>
+      </c>
+      <c r="D52">
+        <v>34.7</v>
+      </c>
+      <c r="E52">
+        <v>37.2</v>
+      </c>
+      <c r="F52">
+        <v>2.9</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>55.7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53">
+        <v>2011</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>-24.5</v>
+      </c>
+      <c r="D53">
+        <v>-22.7</v>
+      </c>
+      <c r="E53">
+        <v>-25.6</v>
+      </c>
+      <c r="F53">
+        <v>-12.4</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>-33.3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>14.3</v>
+      </c>
+      <c r="D54">
+        <v>15.1</v>
+      </c>
+      <c r="E54">
+        <v>13.4</v>
+      </c>
+      <c r="F54">
+        <v>19.2</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>26.3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55">
+        <v>-6.4</v>
+      </c>
+      <c r="D55">
+        <v>-7.1</v>
+      </c>
+      <c r="E55">
+        <v>-9.9</v>
+      </c>
+      <c r="F55">
+        <v>-17.3</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>-2.3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56">
+        <v>30.8</v>
+      </c>
+      <c r="D56">
+        <v>30.6</v>
+      </c>
+      <c r="E56">
+        <v>37.3</v>
+      </c>
+      <c r="F56">
+        <v>40.4</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>45.8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="A57">
+        <v>2012</v>
+      </c>
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57">
+        <v>-16</v>
+      </c>
+      <c r="D57">
+        <v>-12</v>
+      </c>
+      <c r="E57">
+        <v>-24.5</v>
+      </c>
+      <c r="F57">
+        <v>-18.5</v>
+      </c>
+      <c r="G57">
+        <v>-28.3</v>
+      </c>
+      <c r="H57">
+        <v>-32.1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58">
+        <v>3.4</v>
+      </c>
+      <c r="D58">
+        <v>10.3</v>
+      </c>
+      <c r="E58">
+        <v>8</v>
+      </c>
+      <c r="F58">
+        <v>5.9</v>
+      </c>
+      <c r="G58">
+        <v>13.9</v>
+      </c>
+      <c r="H58">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59">
+        <v>-6.4</v>
+      </c>
+      <c r="D59">
+        <v>-2.9</v>
+      </c>
+      <c r="E59">
+        <v>-3.4</v>
+      </c>
+      <c r="F59">
+        <v>-0.9</v>
+      </c>
+      <c r="G59">
+        <v>-5.7</v>
+      </c>
+      <c r="H59">
+        <v>-5.9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60">
+        <v>30.3</v>
+      </c>
+      <c r="D60">
+        <v>29.8</v>
+      </c>
+      <c r="E60">
+        <v>38.3</v>
+      </c>
+      <c r="F60">
+        <v>33.3</v>
+      </c>
+      <c r="G60">
+        <v>39.5</v>
+      </c>
+      <c r="H60">
+        <v>36.1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
+      <c r="A61">
+        <v>2013</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61">
+        <v>-18.8</v>
+      </c>
+      <c r="D61">
+        <v>-23.4</v>
+      </c>
+      <c r="E61">
+        <v>-29.5</v>
+      </c>
+      <c r="F61">
+        <v>-21.1</v>
+      </c>
+      <c r="G61">
+        <v>-25.9</v>
+      </c>
+      <c r="H61">
+        <v>-32.4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62">
+        <v>7.7</v>
+      </c>
+      <c r="D62">
+        <v>9.6</v>
+      </c>
+      <c r="E62">
+        <v>8.7</v>
+      </c>
+      <c r="F62">
+        <v>21.3</v>
+      </c>
+      <c r="G62">
+        <v>17.7</v>
+      </c>
+      <c r="H62">
+        <v>22.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>